<commit_message>
1.1.0 - agregar hoja
</commit_message>
<xml_diff>
--- a/datasets/prueba.xlsx
+++ b/datasets/prueba.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,48 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\2019\Inteligencia Artificial\TPI\decisiontree\tpi\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7801CC11-FCFF-42F2-AEF1-B3D4C354C156}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D63EAE16-7C96-4306-BFD3-5F091F348B76}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="prueba" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>2,2,1</t>
-  </si>
-  <si>
-    <t>2,7,0</t>
-  </si>
-  <si>
-    <t>2,6,0</t>
-  </si>
-  <si>
-    <t>2,8,0</t>
-  </si>
-  <si>
-    <t>7,2,0</t>
-  </si>
-  <si>
-    <t>6,2,0</t>
-  </si>
-  <si>
-    <t>6.5,2,0</t>
-  </si>
-  <si>
-    <t>6.6,2,0</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -883,10 +862,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:A321"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A301" workbookViewId="0">
+      <selection activeCell="A204" sqref="A204:A321"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -895,48 +876,1928 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
-        <f ca="1">CONCATENATE(RANDBETWEEN(1,1000),",",RANDBETWEEN(1,500),",",RANDBETWEEN(0,1))</f>
-        <v>299,116,1</v>
+        <f ca="1">CONCATENATE(RANDBETWEEN(1,200),",",RANDBETWEEN(1,200),",",1)</f>
+        <v>195,180,1</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
+      <c r="A2" t="str">
+        <f t="shared" ref="A2:A49" ca="1" si="0">CONCATENATE(RANDBETWEEN(1,200),",",RANDBETWEEN(1,200),",",1)</f>
+        <v>172,40,1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
+      <c r="A3" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>11,52,1</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
+      <c r="A4" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>7,143,1</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
+      <c r="A5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>13,169,1</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>4</v>
+      <c r="A6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>197,193,1</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>5</v>
+      <c r="A7" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>156,157,1</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>6</v>
+      <c r="A8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>194,119,1</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>7</v>
+      <c r="A9" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>149,102,1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>55,76,1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>33,120,1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>14,186,1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>136,139,1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>172,61,1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>114,130,1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>143,196,1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>78,141,1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>94,130,1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>43,170,1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>49,51,1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>99,129,1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>53,23,1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>6,162,1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>164,102,1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>117,200,1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>104,152,1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>77,5,1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>195,159,1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>74,119,1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>177,189,1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>91,80,1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>104,136,1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>84,72,1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>89,101,1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>88,136,1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>188,82,1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>148,6,1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>83,183,1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>97,151,1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>25,40,1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>145,163,1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>174,77,1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>117,134,1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>163,192,1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>155,84,1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>15,70,1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>198,57,1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>31,108,1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>122,138,1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="str">
+        <f ca="1">CONCATENATE(RANDBETWEEN(200,400),",",RANDBETWEEN(200,400),",",0)</f>
+        <v>337,246,0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="str">
+        <f t="shared" ref="A51:A114" ca="1" si="1">CONCATENATE(RANDBETWEEN(200,400),",",RANDBETWEEN(200,400),",",0)</f>
+        <v>226,229,0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>336,334,0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>249,241,0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>332,263,0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>216,361,0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>327,231,0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>387,212,0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>354,220,0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>208,291,0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>310,241,0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>270,248,0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>346,307,0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>330,344,0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>274,345,0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>388,342,0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>376,257,0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>212,251,0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>339,374,0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>309,261,0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>293,307,0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>307,238,0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>275,288,0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>277,256,0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>289,352,0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>232,384,0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>201,246,0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>330,292,0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>368,293,0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>326,218,0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>276,210,0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>226,238,0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>217,291,0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>202,213,0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>257,268,0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>247,343,0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>320,268,0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>333,243,0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>371,369,0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>330,336,0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>272,243,0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>361,344,0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>269,222,0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>365,206,0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>203,216,0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>291,371,0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>345,237,0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>220,276,0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>377,336,0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>233,230,0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>301,354,0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>219,280,0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>326,374,0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>317,246,0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>229,363,0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>256,213,0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>332,250,0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>393,338,0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>224,337,0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>248,225,0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>348,320,0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>343,244,0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>293,383,0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>267,369,0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>249,310,0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" t="str">
+        <f t="shared" ref="A115:A178" ca="1" si="2">CONCATENATE(RANDBETWEEN(200,400),",",RANDBETWEEN(200,400),",",0)</f>
+        <v>284,277,0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>351,273,0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>254,283,0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>245,200,0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>280,269,0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>263,321,0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>376,325,0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>257,365,0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>336,346,0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>300,237,0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>301,269,0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>366,377,0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>227,311,0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>271,214,0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>250,384,0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>207,369,0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>210,301,0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>319,265,0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>358,315,0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>281,239,0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>266,232,0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>274,223,0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>254,326,0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>225,240,0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>348,202,0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>278,334,0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>285,244,0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A142" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>260,283,0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A143" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>227,353,0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>328,279,0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>355,389,0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>368,293,0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>396,335,0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>372,347,0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>380,203,0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>215,228,0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A151" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>221,311,0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A152" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>394,251,0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A153" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>200,330,0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A154" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>387,236,0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>365,383,0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A156" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>285,246,0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A157" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>210,370,0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A158" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>300,244,0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A159" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>380,283,0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A160" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>345,252,0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A161" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>349,216,0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>278,341,0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A163" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>250,285,0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A164" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>244,321,0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A165" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>343,347,0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A166" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>280,226,0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A167" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>293,334,0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A168" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>302,322,0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A169" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>266,215,0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A170" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>204,398,0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A171" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>259,222,0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A172" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>226,200,0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A173" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>378,350,0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A174" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>323,394,0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A175" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>384,353,0</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A176" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>378,277,0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A177" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>202,235,0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A178" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>357,253,0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A179" t="str">
+        <f t="shared" ref="A179:A181" ca="1" si="3">CONCATENATE(RANDBETWEEN(200,400),",",RANDBETWEEN(200,400),",",0)</f>
+        <v>315,317,0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A180" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>377,219,0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A181" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>247,338,0</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A182" t="str">
+        <f ca="1">CONCATENATE(RANDBETWEEN(400,600),",",RANDBETWEEN(400,600),",",1)</f>
+        <v>446,400,1</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A183" t="str">
+        <f t="shared" ref="A183:A246" ca="1" si="4">CONCATENATE(RANDBETWEEN(400,600),",",RANDBETWEEN(400,600),",",1)</f>
+        <v>523,566,1</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A184" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>553,524,1</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A185" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>575,532,1</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A186" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>590,577,1</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A187" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>455,541,1</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A188" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>584,488,1</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A189" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>406,582,1</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A190" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>468,543,1</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A191" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>429,405,1</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A192" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>412,406,1</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A193" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>502,570,1</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A194" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>559,539,1</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A195" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>593,495,1</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A196" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>483,491,1</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A197" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>483,592,1</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A198" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>502,510,1</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A199" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>480,471,1</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A200" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>514,580,1</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A201" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>551,428,1</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A202" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>425,579,1</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A203" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>432,557,1</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A204" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>440,510,1</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A205" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>466,477,1</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A206" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>442,592,1</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A207" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>508,545,1</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A208" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>460,511,1</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A209" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>416,566,1</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A210" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>454,544,1</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A211" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>467,427,1</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A212" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>520,469,1</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A213" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>469,457,1</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A214" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>429,565,1</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A215" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>437,486,1</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A216" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>435,538,1</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A217" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>553,440,1</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A218" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>591,463,1</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A219" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>488,539,1</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A220" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>569,527,1</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A221" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>442,505,1</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A222" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>497,510,1</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A223" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>516,454,1</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A224" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>455,449,1</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A225" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>479,466,1</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A226" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>446,468,1</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A227" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>478,564,1</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A228" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>558,593,1</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A229" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>467,546,1</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A230" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>401,410,1</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A231" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>465,579,1</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A232" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>462,580,1</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A233" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>476,486,1</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A234" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>469,586,1</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A235" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>542,526,1</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A236" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>582,543,1</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A237" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>556,542,1</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A238" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>491,580,1</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A239" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>545,516,1</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A240" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>411,470,1</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A241" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>562,561,1</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A242" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>528,539,1</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A243" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>433,589,1</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A244" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>578,425,1</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A245" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>588,568,1</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A246" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>402,469,1</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A247" t="str">
+        <f t="shared" ref="A247:A310" ca="1" si="5">CONCATENATE(RANDBETWEEN(400,600),",",RANDBETWEEN(400,600),",",1)</f>
+        <v>459,464,1</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A248" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>462,550,1</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A249" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>590,507,1</v>
+      </c>
+    </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A250" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>403,462,1</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A251" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>479,477,1</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A252" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>528,407,1</v>
+      </c>
+    </row>
+    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A253" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>536,500,1</v>
+      </c>
+    </row>
+    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A254" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>509,564,1</v>
+      </c>
+    </row>
+    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A255" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>597,532,1</v>
+      </c>
+    </row>
+    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A256" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>523,559,1</v>
+      </c>
+    </row>
+    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A257" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>595,414,1</v>
+      </c>
+    </row>
+    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A258" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>580,502,1</v>
+      </c>
+    </row>
+    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A259" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>457,517,1</v>
+      </c>
+    </row>
+    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A260" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>452,501,1</v>
+      </c>
+    </row>
+    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A261" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>561,410,1</v>
+      </c>
+    </row>
+    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A262" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>419,513,1</v>
+      </c>
+    </row>
+    <row r="263" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A263" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>541,452,1</v>
+      </c>
+    </row>
+    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A264" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>556,529,1</v>
+      </c>
+    </row>
+    <row r="265" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A265" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>465,568,1</v>
+      </c>
+    </row>
+    <row r="266" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A266" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>556,431,1</v>
+      </c>
+    </row>
+    <row r="267" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A267" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>430,586,1</v>
+      </c>
+    </row>
+    <row r="268" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A268" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>407,412,1</v>
+      </c>
+    </row>
+    <row r="269" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A269" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>467,529,1</v>
+      </c>
+    </row>
+    <row r="270" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A270" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>588,474,1</v>
+      </c>
+    </row>
+    <row r="271" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A271" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>435,548,1</v>
+      </c>
+    </row>
+    <row r="272" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A272" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>587,438,1</v>
+      </c>
+    </row>
+    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A273" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>471,489,1</v>
+      </c>
+    </row>
+    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A274" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>446,445,1</v>
+      </c>
+    </row>
+    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A275" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>533,500,1</v>
+      </c>
+    </row>
+    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A276" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>563,495,1</v>
+      </c>
+    </row>
+    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A277" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>582,592,1</v>
+      </c>
+    </row>
+    <row r="278" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A278" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>567,480,1</v>
+      </c>
+    </row>
+    <row r="279" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A279" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>513,558,1</v>
+      </c>
+    </row>
+    <row r="280" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A280" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>466,443,1</v>
+      </c>
+    </row>
+    <row r="281" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A281" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>465,600,1</v>
+      </c>
+    </row>
+    <row r="282" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A282" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>484,576,1</v>
+      </c>
+    </row>
+    <row r="283" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A283" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>483,546,1</v>
+      </c>
+    </row>
+    <row r="284" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A284" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>597,588,1</v>
+      </c>
+    </row>
+    <row r="285" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A285" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>458,470,1</v>
+      </c>
+    </row>
+    <row r="286" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A286" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>513,587,1</v>
+      </c>
+    </row>
+    <row r="287" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A287" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>526,453,1</v>
+      </c>
+    </row>
+    <row r="288" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A288" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>405,597,1</v>
+      </c>
+    </row>
+    <row r="289" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A289" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>562,453,1</v>
+      </c>
+    </row>
+    <row r="290" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A290" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>416,592,1</v>
+      </c>
+    </row>
+    <row r="291" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A291" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>561,437,1</v>
+      </c>
+    </row>
+    <row r="292" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A292" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>475,542,1</v>
+      </c>
+    </row>
+    <row r="293" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A293" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>416,581,1</v>
+      </c>
+    </row>
+    <row r="294" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A294" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>484,409,1</v>
+      </c>
+    </row>
+    <row r="295" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A295" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>531,475,1</v>
+      </c>
+    </row>
+    <row r="296" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A296" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>523,544,1</v>
+      </c>
+    </row>
+    <row r="297" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A297" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>433,557,1</v>
+      </c>
+    </row>
+    <row r="298" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A298" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>467,446,1</v>
+      </c>
+    </row>
+    <row r="299" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A299" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>557,544,1</v>
+      </c>
+    </row>
+    <row r="300" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A300" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>521,465,1</v>
+      </c>
+    </row>
+    <row r="301" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A301" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>477,569,1</v>
+      </c>
+    </row>
+    <row r="302" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A302" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>589,477,1</v>
+      </c>
+    </row>
+    <row r="303" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A303" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>538,523,1</v>
+      </c>
+    </row>
+    <row r="304" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A304" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>467,513,1</v>
+      </c>
+    </row>
+    <row r="305" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A305" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>430,447,1</v>
+      </c>
+    </row>
+    <row r="306" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A306" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>579,461,1</v>
+      </c>
+    </row>
+    <row r="307" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A307" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>505,430,1</v>
+      </c>
+    </row>
+    <row r="308" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A308" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>543,494,1</v>
+      </c>
+    </row>
+    <row r="309" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A309" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>481,580,1</v>
+      </c>
+    </row>
+    <row r="310" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A310" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>478,438,1</v>
+      </c>
+    </row>
+    <row r="311" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A311" t="str">
+        <f t="shared" ref="A311:A321" ca="1" si="6">CONCATENATE(RANDBETWEEN(400,600),",",RANDBETWEEN(400,600),",",1)</f>
+        <v>583,433,1</v>
+      </c>
+    </row>
+    <row r="312" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A312" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>447,521,1</v>
+      </c>
+    </row>
+    <row r="313" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A313" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>583,557,1</v>
+      </c>
+    </row>
+    <row r="314" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A314" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>570,421,1</v>
+      </c>
+    </row>
+    <row r="315" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A315" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>535,454,1</v>
+      </c>
+    </row>
+    <row r="316" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A316" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>559,507,1</v>
+      </c>
+    </row>
+    <row r="317" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A317" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>475,465,1</v>
+      </c>
+    </row>
+    <row r="318" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A318" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>591,580,1</v>
+      </c>
+    </row>
+    <row r="319" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A319" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>406,488,1</v>
+      </c>
+    </row>
+    <row r="320" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A320" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>465,401,1</v>
+      </c>
+    </row>
+    <row r="321" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A321" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>469,575,1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>